<commit_message>
yeah!!!! works well in tensorflow 2
</commit_message>
<xml_diff>
--- a/myYolo/yolo_model_structure.xlsx
+++ b/myYolo/yolo_model_structure.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunjim/machine_learning/playground/myYolo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD9F8C1-2D8D-0C42-A675-BEB90A023228}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388D8A10-BF10-CF4E-B6FC-4974241DCCDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26260" yWindow="-20900" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{F17986B6-8B85-8D41-8DD7-D1262351D502}"/>
+    <workbookView xWindow="3020" yWindow="2480" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{F17986B6-8B85-8D41-8DD7-D1262351D502}"/>
   </bookViews>
   <sheets>
     <sheet name="yolo" sheetId="1" r:id="rId1"/>
     <sheet name="ResNet50" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="model_with_loss" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="369">
   <si>
     <t xml:space="preserve">Layer (type)                     Output Shape          Param #     Connected to                     </t>
   </si>
@@ -882,6 +882,267 @@
   </si>
   <si>
     <t>Non-trainable params: 53,120</t>
+  </si>
+  <si>
+    <t>﻿__________________________________________________________________________________________________</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input_1 (InputLayer)            [(None, 416, 416, 3) 0                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d (Conv2D)                 (None, 416, 416, 32) 864         input_1[0][0]                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization (BatchNorma (None, 416, 416, 32) 128         conv2d[0][0]                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu (LeakyReLU)         (None, 416, 416, 32) 0           batch_normalization[0][0]        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_pooling2d (MaxPooling2D)    (None, 208, 208, 32) 0           leaky_re_lu[0][0]                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_1 (Conv2D)               (None, 208, 208, 64) 18432       max_pooling2d[0][0]              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_1 (BatchNor (None, 208, 208, 64) 256         conv2d_1[0][0]                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_1 (LeakyReLU)       (None, 208, 208, 64) 0           batch_normalization_1[0][0]      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_pooling2d_1 (MaxPooling2D)  (None, 104, 104, 64) 0           leaky_re_lu_1[0][0]              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_2 (Conv2D)               (None, 104, 104, 128 73728       max_pooling2d_1[0][0]            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_2 (BatchNor (None, 104, 104, 128 512         conv2d_2[0][0]                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_2 (LeakyReLU)       (None, 104, 104, 128 0           batch_normalization_2[0][0]      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_3 (Conv2D)               (None, 104, 104, 64) 8192        leaky_re_lu_2[0][0]              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_3 (BatchNor (None, 104, 104, 64) 256         conv2d_3[0][0]                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_3 (LeakyReLU)       (None, 104, 104, 64) 0           batch_normalization_3[0][0]      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_4 (Conv2D)               (None, 104, 104, 128 73728       leaky_re_lu_3[0][0]              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_4 (BatchNor (None, 104, 104, 128 512         conv2d_4[0][0]                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_4 (LeakyReLU)       (None, 104, 104, 128 0           batch_normalization_4[0][0]      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_pooling2d_2 (MaxPooling2D)  (None, 52, 52, 128)  0           leaky_re_lu_4[0][0]              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_5 (Conv2D)               (None, 52, 52, 256)  294912      max_pooling2d_2[0][0]            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_5 (BatchNor (None, 52, 52, 256)  1024        conv2d_5[0][0]                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_5 (LeakyReLU)       (None, 52, 52, 256)  0           batch_normalization_5[0][0]      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_6 (Conv2D)               (None, 52, 52, 128)  32768       leaky_re_lu_5[0][0]              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_6 (BatchNor (None, 52, 52, 128)  512         conv2d_6[0][0]                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_6 (LeakyReLU)       (None, 52, 52, 128)  0           batch_normalization_6[0][0]      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_7 (Conv2D)               (None, 52, 52, 256)  294912      leaky_re_lu_6[0][0]              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_7 (BatchNor (None, 52, 52, 256)  1024        conv2d_7[0][0]                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_7 (LeakyReLU)       (None, 52, 52, 256)  0           batch_normalization_7[0][0]      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_pooling2d_3 (MaxPooling2D)  (None, 26, 26, 256)  0           leaky_re_lu_7[0][0]              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_8 (Conv2D)               (None, 26, 26, 512)  1179648     max_pooling2d_3[0][0]            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_8 (BatchNor (None, 26, 26, 512)  2048        conv2d_8[0][0]                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_8 (LeakyReLU)       (None, 26, 26, 512)  0           batch_normalization_8[0][0]      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_9 (Conv2D)               (None, 26, 26, 256)  131072      leaky_re_lu_8[0][0]              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_9 (BatchNor (None, 26, 26, 256)  1024        conv2d_9[0][0]                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_9 (LeakyReLU)       (None, 26, 26, 256)  0           batch_normalization_9[0][0]      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_10 (Conv2D)              (None, 26, 26, 512)  1179648     leaky_re_lu_9[0][0]              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_10 (BatchNo (None, 26, 26, 512)  2048        conv2d_10[0][0]                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_10 (LeakyReLU)      (None, 26, 26, 512)  0           batch_normalization_10[0][0]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_11 (Conv2D)              (None, 26, 26, 256)  131072      leaky_re_lu_10[0][0]             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_11 (BatchNo (None, 26, 26, 256)  1024        conv2d_11[0][0]                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_11 (LeakyReLU)      (None, 26, 26, 256)  0           batch_normalization_11[0][0]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_12 (Conv2D)              (None, 26, 26, 512)  1179648     leaky_re_lu_11[0][0]             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_12 (BatchNo (None, 26, 26, 512)  2048        conv2d_12[0][0]                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_12 (LeakyReLU)      (None, 26, 26, 512)  0           batch_normalization_12[0][0]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_pooling2d_4 (MaxPooling2D)  (None, 13, 13, 512)  0           leaky_re_lu_12[0][0]             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_13 (Conv2D)              (None, 13, 13, 1024) 4718592     max_pooling2d_4[0][0]            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_13 (BatchNo (None, 13, 13, 1024) 4096        conv2d_13[0][0]                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_13 (LeakyReLU)      (None, 13, 13, 1024) 0           batch_normalization_13[0][0]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_14 (Conv2D)              (None, 13, 13, 512)  524288      leaky_re_lu_13[0][0]             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_14 (BatchNo (None, 13, 13, 512)  2048        conv2d_14[0][0]                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_14 (LeakyReLU)      (None, 13, 13, 512)  0           batch_normalization_14[0][0]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_15 (Conv2D)              (None, 13, 13, 1024) 4718592     leaky_re_lu_14[0][0]             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_15 (BatchNo (None, 13, 13, 1024) 4096        conv2d_15[0][0]                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_15 (LeakyReLU)      (None, 13, 13, 1024) 0           batch_normalization_15[0][0]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_16 (Conv2D)              (None, 13, 13, 512)  524288      leaky_re_lu_15[0][0]             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_16 (BatchNo (None, 13, 13, 512)  2048        conv2d_16[0][0]                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_16 (LeakyReLU)      (None, 13, 13, 512)  0           batch_normalization_16[0][0]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_17 (Conv2D)              (None, 13, 13, 1024) 4718592     leaky_re_lu_16[0][0]             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_17 (BatchNo (None, 13, 13, 1024) 4096        conv2d_17[0][0]                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_17 (LeakyReLU)      (None, 13, 13, 1024) 0           batch_normalization_17[0][0]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_18 (Conv2D)              (None, 13, 13, 1024) 9437184     leaky_re_lu_17[0][0]             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_18 (BatchNo (None, 13, 13, 1024) 4096        conv2d_18[0][0]                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_20 (Conv2D)              (None, 26, 26, 64)   32768       leaky_re_lu_12[0][0]             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_18 (LeakyReLU)      (None, 13, 13, 1024) 0           batch_normalization_18[0][0]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_20 (BatchNo (None, 26, 26, 64)   256         conv2d_20[0][0]                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_19 (Conv2D)              (None, 13, 13, 1024) 9437184     leaky_re_lu_18[0][0]             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_20 (LeakyReLU)      (None, 26, 26, 64)   0           batch_normalization_20[0][0]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_19 (BatchNo (None, 13, 13, 1024) 4096        conv2d_19[0][0]                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lambda_space_depth (Lambda)     (None, 13, 13, 256)  0           leaky_re_lu_20[0][0]             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_19 (LeakyReLU)      (None, 13, 13, 1024) 0           batch_normalization_19[0][0]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">concatenate (Concatenate)       (None, 13, 13, 1280) 0           Lambda_space_depth[0][0]         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                 leaky_re_lu_19[0][0]             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_21 (Conv2D)              (None, 13, 13, 1024) 11796480    concatenate[0][0]                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_normalization_21 (BatchNo (None, 13, 13, 1024) 4096        conv2d_21[0][0]                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky_re_lu_21 (LeakyReLU)      (None, 13, 13, 1024) 0           batch_normalization_21[0][0]     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conv2d_23 (Conv2D)              (None, 13, 13, 125)  128125      leaky_re_lu_21[0][0]             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">input_2 (InputLayer)            [(None, None, 5)]    0                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">input_3 (InputLayer)            [(None, 13, 13, 5, 1 0                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">input_4 (InputLayer)            [(None, 13, 13, 5, 5 0                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">yolo_loss (Lambda)              ()                   0           conv2d_23[0][0]                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                 input_2[0][0]                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                 input_3[0][0]                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                 input_4[0][0]                    </t>
+  </si>
+  <si>
+    <t>Total params: 50,676,061</t>
+  </si>
+  <si>
+    <t>Trainable params: 128,125</t>
+  </si>
+  <si>
+    <t>Non-trainable params: 50,547,936</t>
   </si>
 </sst>
 </file>
@@ -1250,7 +1511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{570F18DD-C56D-2744-AF81-6FC5BB220752}">
   <dimension ref="B1:B157"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A132" workbookViewId="0">
       <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
@@ -3957,12 +4218,860 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61041479-DF82-E14D-8FDC-9A8C832D7870}">
-  <dimension ref="A1"/>
+  <dimension ref="B3:B171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B171"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B80" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B82" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B83" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B84" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B85" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B86" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B90" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B91" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B92" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B94" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B95" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B98" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B99" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B100" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B101" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B102" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B104" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B105" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B106" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B107" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B108" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B110" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B111" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B112" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B113" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B114" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B115" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B116" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B117" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B118" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B119" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B120" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B121" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B122" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B123" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B124" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B125" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B126" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B127" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B128" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B129" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B130" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B131" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B132" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B133" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B134" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B135" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B136" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B137" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B138" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B139" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B140" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B141" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B142" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B143" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B144" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B145" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B146" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B147" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B148" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B149" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B150" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B151" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B152" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B153" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B154" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B155" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B156" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B157" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B158" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B159" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B160" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B161" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B162" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B163" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B164" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B165" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B166" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B167" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B168" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B169" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="170" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B170" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="171" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B171" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>